<commit_message>
Salva as predições do PCR (em dados com SNV) no formato XLSX
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_snv.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_snv.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6983202269052741</v>
+        <v>0.6983202269055727</v>
       </c>
       <c r="D2" t="n">
-        <v>4.198865276153277</v>
+        <v>4.19886527614913</v>
       </c>
       <c r="E2" t="n">
-        <v>1.429581063127449</v>
+        <v>1.429581063126747</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6983202269052755</v>
+        <v>0.6983202269055722</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6896071285762483</v>
+        <v>0.6896071285765546</v>
       </c>
       <c r="D3" t="n">
-        <v>4.325757900201753</v>
+        <v>4.325757900197462</v>
       </c>
       <c r="E3" t="n">
-        <v>1.472501160107113</v>
+        <v>1.472501160106388</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6799337285634935</v>
+        <v>0.679933728563809</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4200686495511044</v>
+        <v>0.4200685572530367</v>
       </c>
       <c r="D4" t="n">
-        <v>1.914545593650809</v>
+        <v>1.914545898357321</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2384655753110454</v>
+        <v>0.2384655942873526</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4200686495511047</v>
+        <v>0.4200685572530369</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3795650414806654</v>
+        <v>0.3795649347936007</v>
       </c>
       <c r="D5" t="n">
-        <v>2.047327540906123</v>
+        <v>2.047327891980246</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2576036263584222</v>
+        <v>0.2576036505720172</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3232486283749658</v>
+        <v>0.3232485011517222</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4443415628889881</v>
+        <v>0.4443415628876685</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6253411803158021</v>
+        <v>0.625341180317287</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4168251714799937</v>
+        <v>0.4168251714804886</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4443415628889883</v>
+        <v>0.4443415628876689</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4238434392714761</v>
+        <v>0.4238434392702012</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6487759254432088</v>
+        <v>0.6487759254446265</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4348087519200772</v>
+        <v>0.4348087519205488</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3953603931606616</v>
+        <v>0.3953603931593501</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4957164145394055</v>
+        <v>0.4957164143343495</v>
       </c>
       <c r="D8" t="n">
-        <v>259.2674177679521</v>
+        <v>259.2674178733775</v>
       </c>
       <c r="E8" t="n">
-        <v>71.78687271822851</v>
+        <v>71.78687273282378</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4957164145394057</v>
+        <v>0.4957164143343502</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4726041602485209</v>
+        <v>0.4726041600223095</v>
       </c>
       <c r="D9" t="n">
-        <v>271.175374807682</v>
+        <v>271.1753749264269</v>
       </c>
       <c r="E9" t="n">
-        <v>75.80335334505658</v>
+        <v>75.80335336996426</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4377083950945739</v>
+        <v>0.4377083947250553</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.620436667246156</v>
+        <v>0.6204366672464389</v>
       </c>
       <c r="D10" t="n">
-        <v>5.798142536333241</v>
+        <v>5.798142536328919</v>
       </c>
       <c r="E10" t="n">
-        <v>1.93856110749302</v>
+        <v>1.938561107492297</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6204366672461562</v>
+        <v>0.620436667246439</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6067678920334776</v>
+        <v>0.6067678920337862</v>
       </c>
       <c r="D11" t="n">
-        <v>6.010205649281278</v>
+        <v>6.01020564927658</v>
       </c>
       <c r="E11" t="n">
-        <v>2.012278428447818</v>
+        <v>2.012278428446951</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5910206280749872</v>
+        <v>0.5910206280753398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Salva as predições do PCR em dados com Standard Normal Variate
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_snv.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_snv.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6983202269055727</v>
+        <v>0.6983202269057159</v>
       </c>
       <c r="D2" t="n">
-        <v>4.19886527614913</v>
+        <v>4.198865276147131</v>
       </c>
       <c r="E2" t="n">
-        <v>1.429581063126747</v>
+        <v>1.429581063126407</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6983202269055722</v>
+        <v>0.6983202269057156</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6896071285765546</v>
+        <v>0.6896071285767009</v>
       </c>
       <c r="D3" t="n">
-        <v>4.325757900197462</v>
+        <v>4.325757900195409</v>
       </c>
       <c r="E3" t="n">
-        <v>1.472501160106388</v>
+        <v>1.472501160106041</v>
       </c>
       <c r="F3" t="n">
-        <v>0.679933728563809</v>
+        <v>0.6799337285639595</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4200685572530367</v>
+        <v>0.4200685799435919</v>
       </c>
       <c r="D4" t="n">
-        <v>1.914545898357321</v>
+        <v>1.914545823448276</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2384655942873526</v>
+        <v>0.2384655896222176</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4200685572530369</v>
+        <v>0.4200685799435925</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3795649347936007</v>
+        <v>0.3795649615256661</v>
       </c>
       <c r="D5" t="n">
-        <v>2.047327891980246</v>
+        <v>2.047327805918666</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2576036505720172</v>
+        <v>0.25760363448408</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3232485011517222</v>
+        <v>0.3232485856810776</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4443415628876685</v>
+        <v>0.4443415628871068</v>
       </c>
       <c r="D6" t="n">
-        <v>0.625341180317287</v>
+        <v>0.625341180317919</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4168251714804886</v>
+        <v>0.4168251714806993</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4443415628876689</v>
+        <v>0.4443415628871071</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4238434392702012</v>
+        <v>0.423843439269651</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6487759254446265</v>
+        <v>0.6487759254452292</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4348087519205488</v>
+        <v>0.4348087519207612</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3953603931593501</v>
+        <v>0.3953603931587593</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4957164143343495</v>
+        <v>0.4957164161127786</v>
       </c>
       <c r="D8" t="n">
-        <v>259.2674178733775</v>
+        <v>259.2674169590336</v>
       </c>
       <c r="E8" t="n">
-        <v>71.78687273282378</v>
+        <v>71.78687260624041</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4957164143343502</v>
+        <v>0.4957164161127787</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4726041600223095</v>
+        <v>0.4726041620261295</v>
       </c>
       <c r="D9" t="n">
-        <v>271.1753749264269</v>
+        <v>271.1753739127643</v>
       </c>
       <c r="E9" t="n">
-        <v>75.80335336996426</v>
+        <v>75.80335324419761</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4377083947250553</v>
+        <v>0.4377083965908708</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6204366672464389</v>
+        <v>0.6204366672459227</v>
       </c>
       <c r="D10" t="n">
-        <v>5.798142536328919</v>
+        <v>5.798142536336802</v>
       </c>
       <c r="E10" t="n">
-        <v>1.938561107492297</v>
+        <v>1.938561107493614</v>
       </c>
       <c r="F10" t="n">
-        <v>0.620436667246439</v>
+        <v>0.6204366672459232</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6067678920337862</v>
+        <v>0.6067678920332961</v>
       </c>
       <c r="D11" t="n">
-        <v>6.01020564927658</v>
+        <v>6.010205649284016</v>
       </c>
       <c r="E11" t="n">
-        <v>2.012278428446951</v>
+        <v>2.012278428448186</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5910206280753398</v>
+        <v>0.5910206280748377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adiciona arquivos com informações do plot do PCR com filtro SNV
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_snv.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_snv.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6983202269057159</v>
+        <v>0.7257523197931459</v>
       </c>
       <c r="D2" t="n">
-        <v>4.198865276147131</v>
+        <v>3.817057569599056</v>
       </c>
       <c r="E2" t="n">
-        <v>1.429581063126407</v>
+        <v>1.363035514247575</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6983202269057156</v>
+        <v>0.7257523197931457</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6896071285767009</v>
+        <v>0.7143413178530797</v>
       </c>
       <c r="D3" t="n">
-        <v>4.325757900195409</v>
+        <v>3.975964136606144</v>
       </c>
       <c r="E3" t="n">
-        <v>1.472501160106041</v>
+        <v>1.462172020271649</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6799337285639595</v>
+        <v>0.6844083110598368</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4200685799435919</v>
+        <v>0.2208274643071332</v>
       </c>
       <c r="D4" t="n">
-        <v>1.914545823448276</v>
+        <v>2.572306780362553</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2384655896222176</v>
+        <v>0.2764102973443819</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4200685799435925</v>
+        <v>0.220827464307133</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3795649615256661</v>
+        <v>0.200350224519713</v>
       </c>
       <c r="D5" t="n">
-        <v>2.047327805918666</v>
+        <v>2.640215549496584</v>
       </c>
       <c r="E5" t="n">
-        <v>0.25760363448408</v>
+        <v>0.2843422165241118</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3232485856810776</v>
+        <v>0.1754672905536122</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4443415628871068</v>
+        <v>0.4463262469701371</v>
       </c>
       <c r="D6" t="n">
-        <v>0.625341180317919</v>
+        <v>0.6231076055098256</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4168251714806993</v>
+        <v>0.4160801037814331</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4443415628871071</v>
+        <v>0.446326246970137</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.423843439269651</v>
+        <v>0.4241068855029057</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6487759254452292</v>
+        <v>0.6482324452444937</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4348087519207612</v>
+        <v>0.4353507314332526</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3953603931587593</v>
+        <v>0.3938521138762955</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4957164161127786</v>
+        <v>0.4351124807044907</v>
       </c>
       <c r="D8" t="n">
-        <v>259.2674169590336</v>
+        <v>290.4257300449753</v>
       </c>
       <c r="E8" t="n">
-        <v>71.78687260624041</v>
+        <v>75.9781313613845</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4957164161127787</v>
+        <v>0.435112480704491</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4726041620261295</v>
+        <v>0.415339100968617</v>
       </c>
       <c r="D9" t="n">
-        <v>271.1753739127643</v>
+        <v>300.4003350860203</v>
       </c>
       <c r="E9" t="n">
-        <v>75.80335324419761</v>
+        <v>78.77358394294578</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4377083965908708</v>
+        <v>0.3927801320263483</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6204366672459227</v>
+        <v>0.620685364174401</v>
       </c>
       <c r="D10" t="n">
-        <v>5.798142536336802</v>
+        <v>5.794343485914299</v>
       </c>
       <c r="E10" t="n">
-        <v>1.938561107493614</v>
+        <v>1.937925912850309</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6204366672459232</v>
+        <v>0.6206853641744012</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6067678920332961</v>
+        <v>0.6058007273239474</v>
       </c>
       <c r="D11" t="n">
-        <v>6.010205649284016</v>
+        <v>6.027106593323159</v>
       </c>
       <c r="E11" t="n">
-        <v>2.012278428448186</v>
+        <v>2.030112941361703</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5910206280748377</v>
+        <v>0.5837390607199583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>